<commit_message>
excel document is geupdate
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alecv\Desktop\Portfolio_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6764C83C-FC80-4196-BAB3-2A1E95258D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754C9992-3279-4D29-B1F8-22CA092421D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="0" windowWidth="19575" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:N516"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
-      <selection activeCell="N509" sqref="N509"/>
+      <selection activeCell="A516" sqref="A516:N516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Er zijn een paar visualisaties aan toegevoegd
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alecv\Desktop\Portfolio_python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alecv\Desktop\Portfolio Python\Portfolio_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754C9992-3279-4D29-B1F8-22CA092421D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1840125-0425-4C21-BC8A-BF1E955574BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="19575" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Food_Sales" sheetId="2" r:id="rId2"/>
+    <sheet name="Vakanties" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Vakanties!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -234,14 +238,44 @@
   <si>
     <t>Trunk</t>
   </si>
+  <si>
+    <t>18-25</t>
+  </si>
+  <si>
+    <t>noon</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Vakantiebestemming</t>
+  </si>
+  <si>
+    <t>Arriveer datum</t>
+  </si>
+  <si>
+    <t>Vertrek datum</t>
+  </si>
+  <si>
+    <t>Prijs</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Spanje</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="169" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -285,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -293,11 +327,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -307,6 +350,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1102,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005BDA15-6C35-46C2-AE3E-1275E588AC5E}">
   <dimension ref="A1:N516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
-      <selection activeCell="A516" sqref="A516:N516"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25316,20 +25368,51 @@
       </c>
     </row>
     <row r="516" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A516" s="2"/>
-      <c r="B516" s="3"/>
-      <c r="C516" s="3"/>
-      <c r="D516" s="3"/>
-      <c r="E516" s="3"/>
-      <c r="F516" s="3"/>
-      <c r="G516" s="3"/>
-      <c r="H516" s="3"/>
-      <c r="I516" s="3"/>
-      <c r="J516" s="3"/>
-      <c r="K516" s="3"/>
-      <c r="L516" s="5"/>
-      <c r="M516" s="5"/>
-      <c r="N516" s="5"/>
+      <c r="A516" s="2">
+        <v>44741</v>
+      </c>
+      <c r="B516" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C516" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D516" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E516" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F516" s="3">
+        <v>1</v>
+      </c>
+      <c r="G516" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H516" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I516" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J516" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K516" s="3">
+        <v>707</v>
+      </c>
+      <c r="L516" s="5" t="str">
+        <f>TEXT(SafetyData[[#This Row],[Date]],"ddd")</f>
+        <v>wo</v>
+      </c>
+      <c r="M516" s="5">
+        <f>MONTH(SafetyData[[#This Row],[Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="N516" s="5">
+        <f>YEAR(SafetyData[[#This Row],[Date]])</f>
+        <v>2022</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -25338,4 +25421,58 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC88D691-2A60-4BFC-956D-E6B36389F305}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="9">
+        <v>37341</v>
+      </c>
+      <c r="E2" s="10">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{EC88D691-2A60-4BFC-956D-E6B36389F305}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Vakantie's en visualisatie daarvan gemapped
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alecv\Desktop\Portfolio Python\Portfolio_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1840125-0425-4C21-BC8A-BF1E955574BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10C18A2-EF4D-4F31-A4B0-3D8E3F21B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14580" yWindow="0" windowWidth="14220" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4156" uniqueCount="84">
   <si>
     <t>Date</t>
   </si>
@@ -260,24 +260,50 @@
     <t>Prijs</t>
   </si>
   <si>
-    <t>Barcelona</t>
+    <t>Spanje</t>
   </si>
   <si>
-    <t>Spanje</t>
+    <t>Mallorca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italië </t>
+  </si>
+  <si>
+    <t>Milaan</t>
+  </si>
+  <si>
+    <t>Italië</t>
+  </si>
+  <si>
+    <t>Venetië</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>https://www.vakantiediscounter.nl/italie/lombardije/milaan/b_b_hotel_milano_cenisio_garibaldi?trip_duration=5&amp;trip_duration_range=2-5&amp;flexibility=2&amp;searchResultUrl=aHR0cHM6Ly93d3cudmFrYW50aWVkaXNjb3VudGVyLm5sL3N0ZWRlbnRyaXAtbWlsYWFuP29yaWdpbj0lMkZzdGVkZW50cmlwLW1pbGFhbiZjaXR5PW1pbGFhbiZob2xpZGF5dHlwZT1jaXR5JnRyaXBfZHVyYXRpb249NSZ0cmlwX2R1cmF0aW9uX3JhbmdlPTItNSZjb3VudHJ5Y29kZT1JVCZmbGV4aWJpbGl0eT0yJnNvcnQ9cHJpY2VfYXNjJnRyYW5zcG9ydHR5cGU9VkwmbGF5b3V0PWxpc3Qmcm9vbT0yXzBfMCZwYWdlPTEmZGVwYXJ0dXJlYWlycG9ydD1BTVN-RUlOflJUTSZkZXBhcnR1cmVkYXRlPTIwMjItMDMtMzEmbGl2ZT10cnVlJmZhY2V0cz1ub2RhdGU.&amp;transporttype=VL&amp;accoid=f2253bb6-4292-4128-a7c0-49403f565f19&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-04-21&amp;live=true</t>
+  </si>
+  <si>
+    <t>https://www.vakantiediscounter.nl/italie/lombardije/milaan/b_b_hotel_milano_cenisio_garibaldi?trip_duration=5&amp;trip_duration_range=2-5&amp;flexibility=2&amp;searchResultUrl=aHR0cHM6Ly93d3cudmFrYW50aWVkaXNjb3VudGVyLm5sL3N0ZWRlbnRyaXAtbWlsYWFuP29yaWdpbj0lMkZzdGVkZW50cmlwLW1pbGFhbiZjaXR5PW1pbGFhbiZob2xpZGF5dHlwZT1jaXR5JnRyaXBfZHVyYXRpb249NSZ0cmlwX2R1cmF0aW9uX3JhbmdlPTItNSZjb3VudHJ5Y29kZT1JVCZmbGV4aWJpbGl0eT0yJnNvcnQ9cHJpY2VfYXNjJnRyYW5zcG9ydHR5cGU9VkwmbGF5b3V0PWxpc3Qmcm9vbT0yXzBfMCZwYWdlPTEmZGVwYXJ0dXJlYWlycG9ydD1BTVN-RUlOflJUTSZkZXBhcnR1cmVkYXRlPTIwMjItMDMtMzEmbGl2ZT10cnVlJmZhY2V0cz1ub2RhdGU.&amp;transporttype=VL&amp;accoid=f2253bb6-4292-4128-a7c0-49403f565f19&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-03-31&amp;live=true</t>
+  </si>
+  <si>
+    <t>https://www.vakantiediscounter.nl/italie/veneto/venetie/hotel_plaza?trip_duration=5&amp;trip_duration_range=2-5&amp;flexibility=2&amp;transporttype=VL&amp;accoid=06b81377-e792-4626-a819-7a80c4d365fe&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-03-31&amp;live=true</t>
+  </si>
+  <si>
+    <t>https://www.vakantiediscounter.nl/italie/veneto/venetie/hotel_plaza?trip_duration=5&amp;trip_duration_range=2-5&amp;flexibility=2&amp;transporttype=VL&amp;accoid=06b81377-e792-4626-a819-7a80c4d365fe&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-04-07&amp;live=true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="169" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="170" formatCode="[$-413]d/mmm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +326,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -337,10 +371,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -353,14 +388,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -25425,54 +25464,161 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC88D691-2A60-4BFC-956D-E6B36389F305}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="9">
-        <v>37341</v>
-      </c>
-      <c r="E2" s="10">
-        <v>123</v>
+      <c r="C2" s="8">
+        <v>44651</v>
+      </c>
+      <c r="D2" s="8">
+        <v>44656</v>
+      </c>
+      <c r="E2" s="7">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="8">
+        <v>44644</v>
+      </c>
+      <c r="D3" s="8">
+        <v>44648</v>
+      </c>
+      <c r="E3" s="7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="8">
+        <v>44651</v>
+      </c>
+      <c r="D4" s="8">
+        <v>44655</v>
+      </c>
+      <c r="E4" s="7">
+        <v>227</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="8">
+        <v>44672</v>
+      </c>
+      <c r="D5" s="8">
+        <v>44676</v>
+      </c>
+      <c r="E5" s="7">
+        <v>282</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="8">
+        <v>44651</v>
+      </c>
+      <c r="D6" s="8">
+        <v>44655</v>
+      </c>
+      <c r="E6" s="7">
+        <v>181</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="8">
+        <v>44658</v>
+      </c>
+      <c r="D7" s="8">
+        <v>44662</v>
+      </c>
+      <c r="E7" s="7">
+        <v>219</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{EC88D691-2A60-4BFC-956D-E6B36389F305}"/>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" display="https://www.vakantiediscounter.nl/italie/veneto/venetie/hotel_plaza?trip_duration=5&amp;trip_duration_range=2-5&amp;flexibility=2&amp;transporttype=VL&amp;accoid=06b81377-e792-4626-a819-7a80c4d365fe&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-03-31&amp;live=true" xr:uid="{2B6947C5-4542-46CC-80EB-5DB4FB6BC718}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
De website is hierin gemaakt\
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alecv\Desktop\Portfolio Python\Portfolio_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10C18A2-EF4D-4F31-A4B0-3D8E3F21B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855ABA06-07F1-4FCE-93A1-7A70FFA5E5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="0" windowWidth="14220" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4156" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4165" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -292,6 +292,24 @@
   <si>
     <t>https://www.vakantiediscounter.nl/italie/veneto/venetie/hotel_plaza?trip_duration=5&amp;trip_duration_range=2-5&amp;flexibility=2&amp;transporttype=VL&amp;accoid=06b81377-e792-4626-a819-7a80c4d365fe&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-04-07&amp;live=true</t>
   </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>https://www.vakantiediscounter.nl/italie/latium/rome/hotel_nova_domus?trip_duration_range=6-10&amp;flexibility=2&amp;transporttype=VL&amp;accoid=f07e5010-8f5b-11df-a2df-001c42000009&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-03-30&amp;live=true</t>
+  </si>
+  <si>
+    <t>Frankrijk</t>
+  </si>
+  <si>
+    <t>Nice</t>
+  </si>
+  <si>
+    <t>https://www.vakantiediscounter.nl/frankrijk/zuid_frankrijk/nice/best_western_roosevelt?trip_duration_range=6-10&amp;flexibility=2&amp;transporttype=VL&amp;accoid=31d098ba-8cbb-4649-bbea-f4bcd931b50d&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-03-29&amp;live=true</t>
+  </si>
+  <si>
+    <t>https://www.vakantiediscounter.nl/italie/latium/rome/hotel_nova_domus?trip_duration_range=6-10&amp;flexibility=2&amp;transporttype=VL&amp;accoid=f07e5010-8f5b-11df-a2df-001c42000009&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-06-09&amp;live=true</t>
+  </si>
 </sst>
 </file>
 
@@ -300,10 +318,10 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="169" formatCode="&quot;€&quot;\ #,##0.00"/>
-    <numFmt numFmtId="170" formatCode="[$-413]d/mmm;@"/>
+    <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$-413]d/mmm;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,8 +356,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +375,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -371,11 +401,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -388,17 +419,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Goed" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -25464,10 +25499,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC88D691-2A60-4BFC-956D-E6B36389F305}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25613,12 +25648,73 @@
         <v>83</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8">
+        <v>44650</v>
+      </c>
+      <c r="D8">
+        <v>44656</v>
+      </c>
+      <c r="E8">
+        <v>253</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="8">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8">
+        <v>44654</v>
+      </c>
+      <c r="E9" s="7">
+        <v>336</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="13">
+        <v>44721</v>
+      </c>
+      <c r="D10" s="13">
+        <v>44726</v>
+      </c>
+      <c r="E10" s="14">
+        <v>214</v>
+      </c>
+      <c r="F10" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{EC88D691-2A60-4BFC-956D-E6B36389F305}"/>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="https://www.vakantiediscounter.nl/italie/veneto/venetie/hotel_plaza?trip_duration=5&amp;trip_duration_range=2-5&amp;flexibility=2&amp;transporttype=VL&amp;accoid=06b81377-e792-4626-a819-7a80c4d365fe&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-03-31&amp;live=true" xr:uid="{2B6947C5-4542-46CC-80EB-5DB4FB6BC718}"/>
+    <hyperlink ref="F8" r:id="rId2" display="https://www.vakantiediscounter.nl/italie/latium/rome/hotel_nova_domus?trip_duration_range=6-10&amp;flexibility=2&amp;transporttype=VL&amp;accoid=f07e5010-8f5b-11df-a2df-001c42000009&amp;originaldate=2022-03-31&amp;room=2_0_0&amp;departureairport=AMS~EIN~RTM&amp;departuredate=2022-03-30&amp;live=true" xr:uid="{7BCB1424-3739-4DEE-B3D4-91B394656BC3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>